<commit_message>
Update schedule file: Y2_B2526_Respiratory_schedule.xlsx
</commit_message>
<xml_diff>
--- a/modules_schedules/Y2_B2526_Respiratory_schedule.xlsx
+++ b/modules_schedules/Y2_B2526_Respiratory_schedule.xlsx
@@ -463,7 +463,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G108"/>
+  <dimension ref="A1:G123"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -810,7 +810,7 @@
       </c>
       <c r="C10" s="2" t="inlineStr">
         <is>
-          <t>pathology lab/museum</t>
+          <t>parasitology sgd/pos</t>
         </is>
       </c>
       <c r="D10" s="2" t="inlineStr">
@@ -820,16 +820,16 @@
       </c>
       <c r="E10" s="3" t="inlineStr">
         <is>
-          <t>16/11/2025</t>
+          <t>19/11/2025</t>
         </is>
       </c>
       <c r="F10" s="4" t="inlineStr">
         <is>
-          <t>12:00:00</t>
+          <t>10:00:00</t>
         </is>
       </c>
       <c r="G10" s="5" t="n">
-        <v>120</v>
+        <v>90</v>
       </c>
     </row>
     <row r="11">
@@ -850,7 +850,7 @@
       </c>
       <c r="D11" s="6" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E11" s="7" t="inlineStr">
@@ -860,7 +860,7 @@
       </c>
       <c r="F11" s="8" t="inlineStr">
         <is>
-          <t>14:00:00</t>
+          <t>12:00:00</t>
         </is>
       </c>
       <c r="G11" s="9" t="n">
@@ -880,22 +880,22 @@
       </c>
       <c r="C12" s="2" t="inlineStr">
         <is>
-          <t>pharmacology</t>
+          <t>pathology lab/museum</t>
         </is>
       </c>
       <c r="D12" s="2" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E12" s="3" t="inlineStr">
         <is>
-          <t>05/11/2025</t>
+          <t>16/11/2025</t>
         </is>
       </c>
       <c r="F12" s="4" t="inlineStr">
         <is>
-          <t>08:00:00</t>
+          <t>14:00:00</t>
         </is>
       </c>
       <c r="G12" s="5" t="n">
@@ -920,17 +920,17 @@
       </c>
       <c r="D13" s="6" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E13" s="7" t="inlineStr">
         <is>
-          <t>19/11/2025</t>
+          <t>05/11/2025</t>
         </is>
       </c>
       <c r="F13" s="8" t="inlineStr">
         <is>
-          <t>12:00:00</t>
+          <t>08:00:00</t>
         </is>
       </c>
       <c r="G13" s="9" t="n">
@@ -950,22 +950,22 @@
       </c>
       <c r="C14" s="2" t="inlineStr">
         <is>
-          <t>physiology</t>
+          <t>pharmacology</t>
         </is>
       </c>
       <c r="D14" s="2" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E14" s="3" t="inlineStr">
         <is>
-          <t>09/11/2025</t>
+          <t>19/11/2025</t>
         </is>
       </c>
       <c r="F14" s="4" t="inlineStr">
         <is>
-          <t>14:00:00</t>
+          <t>12:00:00</t>
         </is>
       </c>
       <c r="G14" s="5" t="n">
@@ -980,12 +980,12 @@
       </c>
       <c r="B15" s="6" t="inlineStr">
         <is>
-          <t>A2</t>
+          <t>A1</t>
         </is>
       </c>
       <c r="C15" s="6" t="inlineStr">
         <is>
-          <t>anatomy</t>
+          <t>physiology</t>
         </is>
       </c>
       <c r="D15" s="6" t="inlineStr">
@@ -995,12 +995,12 @@
       </c>
       <c r="E15" s="7" t="inlineStr">
         <is>
-          <t>23/10/2025</t>
+          <t>09/11/2025</t>
         </is>
       </c>
       <c r="F15" s="8" t="inlineStr">
         <is>
-          <t>12:00:00</t>
+          <t>14:00:00</t>
         </is>
       </c>
       <c r="G15" s="9" t="n">
@@ -1015,12 +1015,12 @@
       </c>
       <c r="B16" s="2" t="inlineStr">
         <is>
-          <t>A2</t>
+          <t>A1</t>
         </is>
       </c>
       <c r="C16" s="2" t="inlineStr">
         <is>
-          <t>anatomy</t>
+          <t>physiology</t>
         </is>
       </c>
       <c r="D16" s="2" t="inlineStr">
@@ -1030,7 +1030,7 @@
       </c>
       <c r="E16" s="3" t="inlineStr">
         <is>
-          <t>30/10/2025</t>
+          <t>19/11/2025</t>
         </is>
       </c>
       <c r="F16" s="4" t="inlineStr">
@@ -1039,7 +1039,7 @@
         </is>
       </c>
       <c r="G16" s="5" t="n">
-        <v>120</v>
+        <v>90</v>
       </c>
     </row>
     <row r="17">
@@ -1060,17 +1060,17 @@
       </c>
       <c r="D17" s="6" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E17" s="7" t="inlineStr">
         <is>
-          <t>13/11/2025</t>
+          <t>23/10/2025</t>
         </is>
       </c>
       <c r="F17" s="8" t="inlineStr">
         <is>
-          <t>10:00:00</t>
+          <t>12:00:00</t>
         </is>
       </c>
       <c r="G17" s="9" t="n">
@@ -1090,22 +1090,22 @@
       </c>
       <c r="C18" s="2" t="inlineStr">
         <is>
-          <t>biochemistry lab/cbl</t>
+          <t>anatomy</t>
         </is>
       </c>
       <c r="D18" s="2" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E18" s="3" t="inlineStr">
         <is>
-          <t>09/11/2025</t>
+          <t>30/10/2025</t>
         </is>
       </c>
       <c r="F18" s="4" t="inlineStr">
         <is>
-          <t>14:00:00</t>
+          <t>10:00:00</t>
         </is>
       </c>
       <c r="G18" s="5" t="n">
@@ -1125,17 +1125,17 @@
       </c>
       <c r="C19" s="6" t="inlineStr">
         <is>
-          <t>biochemistry lab/cbl</t>
+          <t>anatomy</t>
         </is>
       </c>
       <c r="D19" s="6" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E19" s="7" t="inlineStr">
         <is>
-          <t>19/11/2025</t>
+          <t>13/11/2025</t>
         </is>
       </c>
       <c r="F19" s="8" t="inlineStr">
@@ -1160,7 +1160,7 @@
       </c>
       <c r="C20" s="2" t="inlineStr">
         <is>
-          <t>histology</t>
+          <t>biochemistry lab/cbl</t>
         </is>
       </c>
       <c r="D20" s="2" t="inlineStr">
@@ -1170,7 +1170,7 @@
       </c>
       <c r="E20" s="3" t="inlineStr">
         <is>
-          <t>23/10/2025</t>
+          <t>09/11/2025</t>
         </is>
       </c>
       <c r="F20" s="4" t="inlineStr">
@@ -1195,7 +1195,7 @@
       </c>
       <c r="C21" s="6" t="inlineStr">
         <is>
-          <t>histology</t>
+          <t>biochemistry lab/cbl</t>
         </is>
       </c>
       <c r="D21" s="6" t="inlineStr">
@@ -1210,7 +1210,7 @@
       </c>
       <c r="F21" s="8" t="inlineStr">
         <is>
-          <t>12:00:00</t>
+          <t>10:00:00</t>
         </is>
       </c>
       <c r="G21" s="9" t="n">
@@ -1230,7 +1230,7 @@
       </c>
       <c r="C22" s="2" t="inlineStr">
         <is>
-          <t>microbiology</t>
+          <t>histology</t>
         </is>
       </c>
       <c r="D22" s="2" t="inlineStr">
@@ -1240,12 +1240,12 @@
       </c>
       <c r="E22" s="3" t="inlineStr">
         <is>
-          <t>10/11/2025</t>
+          <t>23/10/2025</t>
         </is>
       </c>
       <c r="F22" s="4" t="inlineStr">
         <is>
-          <t>08:00:00</t>
+          <t>14:00:00</t>
         </is>
       </c>
       <c r="G22" s="5" t="n">
@@ -1265,22 +1265,22 @@
       </c>
       <c r="C23" s="6" t="inlineStr">
         <is>
-          <t>pathology lab/museum</t>
+          <t>histology</t>
         </is>
       </c>
       <c r="D23" s="6" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E23" s="7" t="inlineStr">
         <is>
-          <t>16/11/2025</t>
+          <t>19/11/2025</t>
         </is>
       </c>
       <c r="F23" s="8" t="inlineStr">
         <is>
-          <t>14:00:00</t>
+          <t>12:00:00</t>
         </is>
       </c>
       <c r="G23" s="9" t="n">
@@ -1300,22 +1300,22 @@
       </c>
       <c r="C24" s="2" t="inlineStr">
         <is>
-          <t>pathology lab/museum</t>
+          <t>microbiology</t>
         </is>
       </c>
       <c r="D24" s="2" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E24" s="3" t="inlineStr">
         <is>
-          <t>16/11/2025</t>
+          <t>10/11/2025</t>
         </is>
       </c>
       <c r="F24" s="4" t="inlineStr">
         <is>
-          <t>12:00:00</t>
+          <t>08:00:00</t>
         </is>
       </c>
       <c r="G24" s="5" t="n">
@@ -1335,7 +1335,7 @@
       </c>
       <c r="C25" s="6" t="inlineStr">
         <is>
-          <t>pharmacology</t>
+          <t>parasitology sgd/pos</t>
         </is>
       </c>
       <c r="D25" s="6" t="inlineStr">
@@ -1345,16 +1345,16 @@
       </c>
       <c r="E25" s="7" t="inlineStr">
         <is>
-          <t>05/11/2025</t>
+          <t>19/11/2025</t>
         </is>
       </c>
       <c r="F25" s="8" t="inlineStr">
         <is>
-          <t>10:00:00</t>
+          <t>08:00:00</t>
         </is>
       </c>
       <c r="G25" s="9" t="n">
-        <v>120</v>
+        <v>90</v>
       </c>
     </row>
     <row r="26">
@@ -1370,17 +1370,17 @@
       </c>
       <c r="C26" s="2" t="inlineStr">
         <is>
-          <t>pharmacology</t>
+          <t>pathology lab/museum</t>
         </is>
       </c>
       <c r="D26" s="2" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E26" s="3" t="inlineStr">
         <is>
-          <t>19/11/2025</t>
+          <t>16/11/2025</t>
         </is>
       </c>
       <c r="F26" s="4" t="inlineStr">
@@ -1405,17 +1405,17 @@
       </c>
       <c r="C27" s="6" t="inlineStr">
         <is>
-          <t>physiology</t>
+          <t>pathology lab/museum</t>
         </is>
       </c>
       <c r="D27" s="6" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E27" s="7" t="inlineStr">
         <is>
-          <t>09/11/2025</t>
+          <t>16/11/2025</t>
         </is>
       </c>
       <c r="F27" s="8" t="inlineStr">
@@ -1435,12 +1435,12 @@
       </c>
       <c r="B28" s="2" t="inlineStr">
         <is>
-          <t>A3</t>
+          <t>A2</t>
         </is>
       </c>
       <c r="C28" s="2" t="inlineStr">
         <is>
-          <t>anatomy</t>
+          <t>pharmacology</t>
         </is>
       </c>
       <c r="D28" s="2" t="inlineStr">
@@ -1450,12 +1450,12 @@
       </c>
       <c r="E28" s="3" t="inlineStr">
         <is>
-          <t>19/10/2025</t>
+          <t>05/11/2025</t>
         </is>
       </c>
       <c r="F28" s="4" t="inlineStr">
         <is>
-          <t>12:00:00</t>
+          <t>10:00:00</t>
         </is>
       </c>
       <c r="G28" s="5" t="n">
@@ -1470,12 +1470,12 @@
       </c>
       <c r="B29" s="6" t="inlineStr">
         <is>
-          <t>A3</t>
+          <t>A2</t>
         </is>
       </c>
       <c r="C29" s="6" t="inlineStr">
         <is>
-          <t>anatomy</t>
+          <t>pharmacology</t>
         </is>
       </c>
       <c r="D29" s="6" t="inlineStr">
@@ -1485,12 +1485,12 @@
       </c>
       <c r="E29" s="7" t="inlineStr">
         <is>
-          <t>01/11/2025</t>
+          <t>19/11/2025</t>
         </is>
       </c>
       <c r="F29" s="8" t="inlineStr">
         <is>
-          <t>08:00:00</t>
+          <t>14:00:00</t>
         </is>
       </c>
       <c r="G29" s="9" t="n">
@@ -1505,27 +1505,27 @@
       </c>
       <c r="B30" s="2" t="inlineStr">
         <is>
-          <t>A3</t>
+          <t>A2</t>
         </is>
       </c>
       <c r="C30" s="2" t="inlineStr">
         <is>
-          <t>anatomy</t>
+          <t>physiology</t>
         </is>
       </c>
       <c r="D30" s="2" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E30" s="3" t="inlineStr">
         <is>
-          <t>26/10/2025</t>
+          <t>09/11/2025</t>
         </is>
       </c>
       <c r="F30" s="4" t="inlineStr">
         <is>
-          <t>14:00:00</t>
+          <t>12:00:00</t>
         </is>
       </c>
       <c r="G30" s="5" t="n">
@@ -1540,31 +1540,31 @@
       </c>
       <c r="B31" s="6" t="inlineStr">
         <is>
-          <t>A3</t>
+          <t>A2</t>
         </is>
       </c>
       <c r="C31" s="6" t="inlineStr">
         <is>
-          <t>anatomy</t>
+          <t>physiology</t>
         </is>
       </c>
       <c r="D31" s="6" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E31" s="7" t="inlineStr">
         <is>
-          <t>11/11/2025</t>
+          <t>19/11/2025</t>
         </is>
       </c>
       <c r="F31" s="8" t="inlineStr">
         <is>
-          <t>12:00:00</t>
+          <t>08:00:00</t>
         </is>
       </c>
       <c r="G31" s="9" t="n">
-        <v>120</v>
+        <v>90</v>
       </c>
     </row>
     <row r="32">
@@ -1580,7 +1580,7 @@
       </c>
       <c r="C32" s="2" t="inlineStr">
         <is>
-          <t>biochemistry lab/cbl</t>
+          <t>anatomy</t>
         </is>
       </c>
       <c r="D32" s="2" t="inlineStr">
@@ -1590,12 +1590,12 @@
       </c>
       <c r="E32" s="3" t="inlineStr">
         <is>
-          <t>12/11/2025</t>
+          <t>19/10/2025</t>
         </is>
       </c>
       <c r="F32" s="4" t="inlineStr">
         <is>
-          <t>08:00:00</t>
+          <t>12:00:00</t>
         </is>
       </c>
       <c r="G32" s="5" t="n">
@@ -1615,7 +1615,7 @@
       </c>
       <c r="C33" s="6" t="inlineStr">
         <is>
-          <t>biochemistry lab/cbl</t>
+          <t>anatomy</t>
         </is>
       </c>
       <c r="D33" s="6" t="inlineStr">
@@ -1625,12 +1625,12 @@
       </c>
       <c r="E33" s="7" t="inlineStr">
         <is>
-          <t>16/11/2025</t>
+          <t>01/11/2025</t>
         </is>
       </c>
       <c r="F33" s="8" t="inlineStr">
         <is>
-          <t>12:00:00</t>
+          <t>08:00:00</t>
         </is>
       </c>
       <c r="G33" s="9" t="n">
@@ -1650,22 +1650,22 @@
       </c>
       <c r="C34" s="2" t="inlineStr">
         <is>
-          <t>histology</t>
+          <t>anatomy</t>
         </is>
       </c>
       <c r="D34" s="2" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E34" s="3" t="inlineStr">
         <is>
-          <t>27/10/2025</t>
+          <t>26/10/2025</t>
         </is>
       </c>
       <c r="F34" s="4" t="inlineStr">
         <is>
-          <t>08:00:00</t>
+          <t>14:00:00</t>
         </is>
       </c>
       <c r="G34" s="5" t="n">
@@ -1685,22 +1685,22 @@
       </c>
       <c r="C35" s="6" t="inlineStr">
         <is>
-          <t>microbiology</t>
+          <t>anatomy</t>
         </is>
       </c>
       <c r="D35" s="6" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E35" s="7" t="inlineStr">
         <is>
-          <t>12/11/2025</t>
+          <t>11/11/2025</t>
         </is>
       </c>
       <c r="F35" s="8" t="inlineStr">
         <is>
-          <t>10:00:00</t>
+          <t>12:00:00</t>
         </is>
       </c>
       <c r="G35" s="9" t="n">
@@ -1720,22 +1720,22 @@
       </c>
       <c r="C36" s="2" t="inlineStr">
         <is>
-          <t>microbiology</t>
+          <t>biochemistry lab/cbl</t>
         </is>
       </c>
       <c r="D36" s="2" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E36" s="3" t="inlineStr">
         <is>
-          <t>15/11/2025</t>
+          <t>12/11/2025</t>
         </is>
       </c>
       <c r="F36" s="4" t="inlineStr">
         <is>
-          <t>10:00:00</t>
+          <t>08:00:00</t>
         </is>
       </c>
       <c r="G36" s="5" t="n">
@@ -1755,22 +1755,22 @@
       </c>
       <c r="C37" s="6" t="inlineStr">
         <is>
-          <t>pathology lab/museum</t>
+          <t>biochemistry lab/cbl</t>
         </is>
       </c>
       <c r="D37" s="6" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E37" s="7" t="inlineStr">
         <is>
-          <t>18/11/2025</t>
+          <t>16/11/2025</t>
         </is>
       </c>
       <c r="F37" s="8" t="inlineStr">
         <is>
-          <t>08:00:00</t>
+          <t>12:00:00</t>
         </is>
       </c>
       <c r="G37" s="9" t="n">
@@ -1790,22 +1790,22 @@
       </c>
       <c r="C38" s="2" t="inlineStr">
         <is>
-          <t>pathology lab/museum</t>
+          <t>histology</t>
         </is>
       </c>
       <c r="D38" s="2" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E38" s="3" t="inlineStr">
         <is>
-          <t>18/11/2025</t>
+          <t>27/10/2025</t>
         </is>
       </c>
       <c r="F38" s="4" t="inlineStr">
         <is>
-          <t>10:00:00</t>
+          <t>08:00:00</t>
         </is>
       </c>
       <c r="G38" s="5" t="n">
@@ -1825,7 +1825,7 @@
       </c>
       <c r="C39" s="6" t="inlineStr">
         <is>
-          <t>pharmacology</t>
+          <t>microbiology</t>
         </is>
       </c>
       <c r="D39" s="6" t="inlineStr">
@@ -1835,12 +1835,12 @@
       </c>
       <c r="E39" s="7" t="inlineStr">
         <is>
-          <t>06/11/2025</t>
+          <t>12/11/2025</t>
         </is>
       </c>
       <c r="F39" s="8" t="inlineStr">
         <is>
-          <t>08:00:00</t>
+          <t>10:00:00</t>
         </is>
       </c>
       <c r="G39" s="9" t="n">
@@ -1860,7 +1860,7 @@
       </c>
       <c r="C40" s="2" t="inlineStr">
         <is>
-          <t>pharmacology</t>
+          <t>microbiology</t>
         </is>
       </c>
       <c r="D40" s="2" t="inlineStr">
@@ -1870,12 +1870,12 @@
       </c>
       <c r="E40" s="3" t="inlineStr">
         <is>
-          <t>18/11/2025</t>
+          <t>15/11/2025</t>
         </is>
       </c>
       <c r="F40" s="4" t="inlineStr">
         <is>
-          <t>12:00:00</t>
+          <t>10:00:00</t>
         </is>
       </c>
       <c r="G40" s="5" t="n">
@@ -1895,7 +1895,7 @@
       </c>
       <c r="C41" s="6" t="inlineStr">
         <is>
-          <t>physiology</t>
+          <t>parasitology sgd/pos</t>
         </is>
       </c>
       <c r="D41" s="6" t="inlineStr">
@@ -1905,16 +1905,16 @@
       </c>
       <c r="E41" s="7" t="inlineStr">
         <is>
-          <t>11/11/2025</t>
+          <t>17/11/2025</t>
         </is>
       </c>
       <c r="F41" s="8" t="inlineStr">
         <is>
-          <t>14:00:00</t>
+          <t>12:00:00</t>
         </is>
       </c>
       <c r="G41" s="9" t="n">
-        <v>120</v>
+        <v>90</v>
       </c>
     </row>
     <row r="42">
@@ -1925,12 +1925,12 @@
       </c>
       <c r="B42" s="2" t="inlineStr">
         <is>
-          <t>A4</t>
+          <t>A3</t>
         </is>
       </c>
       <c r="C42" s="2" t="inlineStr">
         <is>
-          <t>anatomy</t>
+          <t>pathology lab/museum</t>
         </is>
       </c>
       <c r="D42" s="2" t="inlineStr">
@@ -1940,12 +1940,12 @@
       </c>
       <c r="E42" s="3" t="inlineStr">
         <is>
-          <t>19/10/2025</t>
+          <t>18/11/2025</t>
         </is>
       </c>
       <c r="F42" s="4" t="inlineStr">
         <is>
-          <t>14:00:00</t>
+          <t>08:00:00</t>
         </is>
       </c>
       <c r="G42" s="5" t="n">
@@ -1960,12 +1960,12 @@
       </c>
       <c r="B43" s="6" t="inlineStr">
         <is>
-          <t>A4</t>
+          <t>A3</t>
         </is>
       </c>
       <c r="C43" s="6" t="inlineStr">
         <is>
-          <t>anatomy</t>
+          <t>pathology lab/museum</t>
         </is>
       </c>
       <c r="D43" s="6" t="inlineStr">
@@ -1975,7 +1975,7 @@
       </c>
       <c r="E43" s="7" t="inlineStr">
         <is>
-          <t>01/11/2025</t>
+          <t>18/11/2025</t>
         </is>
       </c>
       <c r="F43" s="8" t="inlineStr">
@@ -1995,27 +1995,27 @@
       </c>
       <c r="B44" s="2" t="inlineStr">
         <is>
-          <t>A4</t>
+          <t>A3</t>
         </is>
       </c>
       <c r="C44" s="2" t="inlineStr">
         <is>
-          <t>anatomy</t>
+          <t>pharmacology</t>
         </is>
       </c>
       <c r="D44" s="2" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E44" s="3" t="inlineStr">
         <is>
-          <t>26/10/2025</t>
+          <t>06/11/2025</t>
         </is>
       </c>
       <c r="F44" s="4" t="inlineStr">
         <is>
-          <t>12:00:00</t>
+          <t>08:00:00</t>
         </is>
       </c>
       <c r="G44" s="5" t="n">
@@ -2030,27 +2030,27 @@
       </c>
       <c r="B45" s="6" t="inlineStr">
         <is>
-          <t>A4</t>
+          <t>A3</t>
         </is>
       </c>
       <c r="C45" s="6" t="inlineStr">
         <is>
-          <t>anatomy</t>
+          <t>pharmacology</t>
         </is>
       </c>
       <c r="D45" s="6" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E45" s="7" t="inlineStr">
         <is>
-          <t>11/11/2025</t>
+          <t>18/11/2025</t>
         </is>
       </c>
       <c r="F45" s="8" t="inlineStr">
         <is>
-          <t>14:00:00</t>
+          <t>12:00:00</t>
         </is>
       </c>
       <c r="G45" s="9" t="n">
@@ -2065,12 +2065,12 @@
       </c>
       <c r="B46" s="2" t="inlineStr">
         <is>
-          <t>A4</t>
+          <t>A3</t>
         </is>
       </c>
       <c r="C46" s="2" t="inlineStr">
         <is>
-          <t>biochemistry lab/cbl</t>
+          <t>physiology</t>
         </is>
       </c>
       <c r="D46" s="2" t="inlineStr">
@@ -2080,12 +2080,12 @@
       </c>
       <c r="E46" s="3" t="inlineStr">
         <is>
-          <t>12/11/2025</t>
+          <t>11/11/2025</t>
         </is>
       </c>
       <c r="F46" s="4" t="inlineStr">
         <is>
-          <t>10:00:00</t>
+          <t>14:00:00</t>
         </is>
       </c>
       <c r="G46" s="5" t="n">
@@ -2100,12 +2100,12 @@
       </c>
       <c r="B47" s="6" t="inlineStr">
         <is>
-          <t>A4</t>
+          <t>A3</t>
         </is>
       </c>
       <c r="C47" s="6" t="inlineStr">
         <is>
-          <t>biochemistry lab/cbl</t>
+          <t>physiology</t>
         </is>
       </c>
       <c r="D47" s="6" t="inlineStr">
@@ -2115,16 +2115,16 @@
       </c>
       <c r="E47" s="7" t="inlineStr">
         <is>
-          <t>16/11/2025</t>
+          <t>17/11/2025</t>
         </is>
       </c>
       <c r="F47" s="8" t="inlineStr">
         <is>
-          <t>14:00:00</t>
+          <t>12:00:00</t>
         </is>
       </c>
       <c r="G47" s="9" t="n">
-        <v>120</v>
+        <v>90</v>
       </c>
     </row>
     <row r="48">
@@ -2140,7 +2140,7 @@
       </c>
       <c r="C48" s="2" t="inlineStr">
         <is>
-          <t>histology</t>
+          <t>anatomy</t>
         </is>
       </c>
       <c r="D48" s="2" t="inlineStr">
@@ -2150,12 +2150,12 @@
       </c>
       <c r="E48" s="3" t="inlineStr">
         <is>
-          <t>27/10/2025</t>
+          <t>19/10/2025</t>
         </is>
       </c>
       <c r="F48" s="4" t="inlineStr">
         <is>
-          <t>10:00:00</t>
+          <t>14:00:00</t>
         </is>
       </c>
       <c r="G48" s="5" t="n">
@@ -2175,22 +2175,22 @@
       </c>
       <c r="C49" s="6" t="inlineStr">
         <is>
-          <t>microbiology</t>
+          <t>anatomy</t>
         </is>
       </c>
       <c r="D49" s="6" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E49" s="7" t="inlineStr">
         <is>
-          <t>12/11/2025</t>
+          <t>01/11/2025</t>
         </is>
       </c>
       <c r="F49" s="8" t="inlineStr">
         <is>
-          <t>08:00:00</t>
+          <t>10:00:00</t>
         </is>
       </c>
       <c r="G49" s="9" t="n">
@@ -2210,7 +2210,7 @@
       </c>
       <c r="C50" s="2" t="inlineStr">
         <is>
-          <t>microbiology</t>
+          <t>anatomy</t>
         </is>
       </c>
       <c r="D50" s="2" t="inlineStr">
@@ -2220,12 +2220,12 @@
       </c>
       <c r="E50" s="3" t="inlineStr">
         <is>
-          <t>15/11/2025</t>
+          <t>26/10/2025</t>
         </is>
       </c>
       <c r="F50" s="4" t="inlineStr">
         <is>
-          <t>08:00:00</t>
+          <t>12:00:00</t>
         </is>
       </c>
       <c r="G50" s="5" t="n">
@@ -2245,22 +2245,22 @@
       </c>
       <c r="C51" s="6" t="inlineStr">
         <is>
-          <t>pathology lab/museum</t>
+          <t>anatomy</t>
         </is>
       </c>
       <c r="D51" s="6" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E51" s="7" t="inlineStr">
         <is>
-          <t>18/11/2025</t>
+          <t>11/11/2025</t>
         </is>
       </c>
       <c r="F51" s="8" t="inlineStr">
         <is>
-          <t>10:00:00</t>
+          <t>14:00:00</t>
         </is>
       </c>
       <c r="G51" s="9" t="n">
@@ -2280,22 +2280,22 @@
       </c>
       <c r="C52" s="2" t="inlineStr">
         <is>
-          <t>pathology lab/museum</t>
+          <t>biochemistry lab/cbl</t>
         </is>
       </c>
       <c r="D52" s="2" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E52" s="3" t="inlineStr">
         <is>
-          <t>18/11/2025</t>
+          <t>12/11/2025</t>
         </is>
       </c>
       <c r="F52" s="4" t="inlineStr">
         <is>
-          <t>08:00:00</t>
+          <t>10:00:00</t>
         </is>
       </c>
       <c r="G52" s="5" t="n">
@@ -2315,22 +2315,22 @@
       </c>
       <c r="C53" s="6" t="inlineStr">
         <is>
-          <t>pharmacology</t>
+          <t>biochemistry lab/cbl</t>
         </is>
       </c>
       <c r="D53" s="6" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E53" s="7" t="inlineStr">
         <is>
-          <t>06/11/2025</t>
+          <t>16/11/2025</t>
         </is>
       </c>
       <c r="F53" s="8" t="inlineStr">
         <is>
-          <t>10:00:00</t>
+          <t>14:00:00</t>
         </is>
       </c>
       <c r="G53" s="9" t="n">
@@ -2350,22 +2350,22 @@
       </c>
       <c r="C54" s="2" t="inlineStr">
         <is>
-          <t>pharmacology</t>
+          <t>histology</t>
         </is>
       </c>
       <c r="D54" s="2" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E54" s="3" t="inlineStr">
         <is>
-          <t>18/11/2025</t>
+          <t>27/10/2025</t>
         </is>
       </c>
       <c r="F54" s="4" t="inlineStr">
         <is>
-          <t>14:00:00</t>
+          <t>10:00:00</t>
         </is>
       </c>
       <c r="G54" s="5" t="n">
@@ -2385,7 +2385,7 @@
       </c>
       <c r="C55" s="6" t="inlineStr">
         <is>
-          <t>physiology</t>
+          <t>microbiology</t>
         </is>
       </c>
       <c r="D55" s="6" t="inlineStr">
@@ -2395,12 +2395,12 @@
       </c>
       <c r="E55" s="7" t="inlineStr">
         <is>
-          <t>11/11/2025</t>
+          <t>12/11/2025</t>
         </is>
       </c>
       <c r="F55" s="8" t="inlineStr">
         <is>
-          <t>12:00:00</t>
+          <t>08:00:00</t>
         </is>
       </c>
       <c r="G55" s="9" t="n">
@@ -2415,27 +2415,27 @@
       </c>
       <c r="B56" s="2" t="inlineStr">
         <is>
-          <t>B1</t>
+          <t>A4</t>
         </is>
       </c>
       <c r="C56" s="2" t="inlineStr">
         <is>
-          <t>anatomy</t>
+          <t>microbiology</t>
         </is>
       </c>
       <c r="D56" s="2" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E56" s="3" t="inlineStr">
         <is>
-          <t>20/10/2025</t>
+          <t>15/11/2025</t>
         </is>
       </c>
       <c r="F56" s="4" t="inlineStr">
         <is>
-          <t>10:00:00</t>
+          <t>08:00:00</t>
         </is>
       </c>
       <c r="G56" s="5" t="n">
@@ -2450,31 +2450,31 @@
       </c>
       <c r="B57" s="6" t="inlineStr">
         <is>
-          <t>B1</t>
+          <t>A4</t>
         </is>
       </c>
       <c r="C57" s="6" t="inlineStr">
         <is>
-          <t>anatomy</t>
+          <t>parasitology sgd/pos</t>
         </is>
       </c>
       <c r="D57" s="6" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E57" s="7" t="inlineStr">
         <is>
-          <t>27/10/2025</t>
+          <t>17/11/2025</t>
         </is>
       </c>
       <c r="F57" s="8" t="inlineStr">
         <is>
-          <t>08:00:00</t>
+          <t>14:00:00</t>
         </is>
       </c>
       <c r="G57" s="9" t="n">
-        <v>120</v>
+        <v>90</v>
       </c>
     </row>
     <row r="58">
@@ -2485,27 +2485,27 @@
       </c>
       <c r="B58" s="2" t="inlineStr">
         <is>
-          <t>B1</t>
+          <t>A4</t>
         </is>
       </c>
       <c r="C58" s="2" t="inlineStr">
         <is>
-          <t>anatomy</t>
+          <t>pathology lab/museum</t>
         </is>
       </c>
       <c r="D58" s="2" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E58" s="3" t="inlineStr">
         <is>
-          <t>12/11/2025</t>
+          <t>18/11/2025</t>
         </is>
       </c>
       <c r="F58" s="4" t="inlineStr">
         <is>
-          <t>12:00:00</t>
+          <t>10:00:00</t>
         </is>
       </c>
       <c r="G58" s="5" t="n">
@@ -2520,22 +2520,22 @@
       </c>
       <c r="B59" s="6" t="inlineStr">
         <is>
-          <t>B1</t>
+          <t>A4</t>
         </is>
       </c>
       <c r="C59" s="6" t="inlineStr">
         <is>
-          <t>biochemistry lab/cbl</t>
+          <t>pathology lab/museum</t>
         </is>
       </c>
       <c r="D59" s="6" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E59" s="7" t="inlineStr">
         <is>
-          <t>10/11/2025</t>
+          <t>18/11/2025</t>
         </is>
       </c>
       <c r="F59" s="8" t="inlineStr">
@@ -2555,27 +2555,27 @@
       </c>
       <c r="B60" s="2" t="inlineStr">
         <is>
-          <t>B1</t>
+          <t>A4</t>
         </is>
       </c>
       <c r="C60" s="2" t="inlineStr">
         <is>
-          <t>biochemistry lab/cbl</t>
+          <t>pharmacology</t>
         </is>
       </c>
       <c r="D60" s="2" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E60" s="3" t="inlineStr">
         <is>
-          <t>18/11/2025</t>
+          <t>06/11/2025</t>
         </is>
       </c>
       <c r="F60" s="4" t="inlineStr">
         <is>
-          <t>08:00:00</t>
+          <t>10:00:00</t>
         </is>
       </c>
       <c r="G60" s="5" t="n">
@@ -2590,27 +2590,27 @@
       </c>
       <c r="B61" s="6" t="inlineStr">
         <is>
-          <t>B1</t>
+          <t>A4</t>
         </is>
       </c>
       <c r="C61" s="6" t="inlineStr">
         <is>
-          <t>histology</t>
+          <t>pharmacology</t>
         </is>
       </c>
       <c r="D61" s="6" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E61" s="7" t="inlineStr">
         <is>
-          <t>22/10/2025</t>
+          <t>18/11/2025</t>
         </is>
       </c>
       <c r="F61" s="8" t="inlineStr">
         <is>
-          <t>12:00:00</t>
+          <t>14:00:00</t>
         </is>
       </c>
       <c r="G61" s="9" t="n">
@@ -2625,27 +2625,27 @@
       </c>
       <c r="B62" s="2" t="inlineStr">
         <is>
-          <t>B1</t>
+          <t>A4</t>
         </is>
       </c>
       <c r="C62" s="2" t="inlineStr">
         <is>
-          <t>histology</t>
+          <t>physiology</t>
         </is>
       </c>
       <c r="D62" s="2" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E62" s="3" t="inlineStr">
         <is>
-          <t>18/11/2025</t>
+          <t>11/11/2025</t>
         </is>
       </c>
       <c r="F62" s="4" t="inlineStr">
         <is>
-          <t>14:00:00</t>
+          <t>12:00:00</t>
         </is>
       </c>
       <c r="G62" s="5" t="n">
@@ -2660,22 +2660,22 @@
       </c>
       <c r="B63" s="6" t="inlineStr">
         <is>
-          <t>B1</t>
+          <t>A4</t>
         </is>
       </c>
       <c r="C63" s="6" t="inlineStr">
         <is>
-          <t>microbiology</t>
+          <t>physiology</t>
         </is>
       </c>
       <c r="D63" s="6" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E63" s="7" t="inlineStr">
         <is>
-          <t>12/11/2025</t>
+          <t>17/11/2025</t>
         </is>
       </c>
       <c r="F63" s="8" t="inlineStr">
@@ -2684,7 +2684,7 @@
         </is>
       </c>
       <c r="G63" s="9" t="n">
-        <v>120</v>
+        <v>90</v>
       </c>
     </row>
     <row r="64">
@@ -2700,7 +2700,7 @@
       </c>
       <c r="C64" s="2" t="inlineStr">
         <is>
-          <t>pathology lab/museum</t>
+          <t>anatomy</t>
         </is>
       </c>
       <c r="D64" s="2" t="inlineStr">
@@ -2710,12 +2710,12 @@
       </c>
       <c r="E64" s="3" t="inlineStr">
         <is>
-          <t>17/11/2025</t>
+          <t>20/10/2025</t>
         </is>
       </c>
       <c r="F64" s="4" t="inlineStr">
         <is>
-          <t>12:00:00</t>
+          <t>10:00:00</t>
         </is>
       </c>
       <c r="G64" s="5" t="n">
@@ -2735,7 +2735,7 @@
       </c>
       <c r="C65" s="6" t="inlineStr">
         <is>
-          <t>pathology lab/museum</t>
+          <t>anatomy</t>
         </is>
       </c>
       <c r="D65" s="6" t="inlineStr">
@@ -2745,12 +2745,12 @@
       </c>
       <c r="E65" s="7" t="inlineStr">
         <is>
-          <t>17/11/2025</t>
+          <t>27/10/2025</t>
         </is>
       </c>
       <c r="F65" s="8" t="inlineStr">
         <is>
-          <t>14:00:00</t>
+          <t>08:00:00</t>
         </is>
       </c>
       <c r="G65" s="9" t="n">
@@ -2770,17 +2770,17 @@
       </c>
       <c r="C66" s="2" t="inlineStr">
         <is>
-          <t>pharmacology</t>
+          <t>anatomy</t>
         </is>
       </c>
       <c r="D66" s="2" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E66" s="3" t="inlineStr">
         <is>
-          <t>05/11/2025</t>
+          <t>12/11/2025</t>
         </is>
       </c>
       <c r="F66" s="4" t="inlineStr">
@@ -2805,17 +2805,17 @@
       </c>
       <c r="C67" s="6" t="inlineStr">
         <is>
-          <t>pharmacology</t>
+          <t>biochemistry lab/cbl</t>
         </is>
       </c>
       <c r="D67" s="6" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E67" s="7" t="inlineStr">
         <is>
-          <t>19/11/2025</t>
+          <t>10/11/2025</t>
         </is>
       </c>
       <c r="F67" s="8" t="inlineStr">
@@ -2840,22 +2840,22 @@
       </c>
       <c r="C68" s="2" t="inlineStr">
         <is>
-          <t>physiology</t>
+          <t>biochemistry lab/cbl</t>
         </is>
       </c>
       <c r="D68" s="2" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E68" s="3" t="inlineStr">
         <is>
-          <t>10/11/2025</t>
+          <t>18/11/2025</t>
         </is>
       </c>
       <c r="F68" s="4" t="inlineStr">
         <is>
-          <t>10:00:00</t>
+          <t>08:00:00</t>
         </is>
       </c>
       <c r="G68" s="5" t="n">
@@ -2870,12 +2870,12 @@
       </c>
       <c r="B69" s="6" t="inlineStr">
         <is>
-          <t>B2</t>
+          <t>B1</t>
         </is>
       </c>
       <c r="C69" s="6" t="inlineStr">
         <is>
-          <t>anatomy</t>
+          <t>histology</t>
         </is>
       </c>
       <c r="D69" s="6" t="inlineStr">
@@ -2885,12 +2885,12 @@
       </c>
       <c r="E69" s="7" t="inlineStr">
         <is>
-          <t>20/10/2025</t>
+          <t>22/10/2025</t>
         </is>
       </c>
       <c r="F69" s="8" t="inlineStr">
         <is>
-          <t>08:00:00</t>
+          <t>12:00:00</t>
         </is>
       </c>
       <c r="G69" s="9" t="n">
@@ -2905,12 +2905,12 @@
       </c>
       <c r="B70" s="2" t="inlineStr">
         <is>
-          <t>B2</t>
+          <t>B1</t>
         </is>
       </c>
       <c r="C70" s="2" t="inlineStr">
         <is>
-          <t>anatomy</t>
+          <t>histology</t>
         </is>
       </c>
       <c r="D70" s="2" t="inlineStr">
@@ -2920,12 +2920,12 @@
       </c>
       <c r="E70" s="3" t="inlineStr">
         <is>
-          <t>30/10/2025</t>
+          <t>18/11/2025</t>
         </is>
       </c>
       <c r="F70" s="4" t="inlineStr">
         <is>
-          <t>08:00:00</t>
+          <t>14:00:00</t>
         </is>
       </c>
       <c r="G70" s="5" t="n">
@@ -2940,27 +2940,27 @@
       </c>
       <c r="B71" s="6" t="inlineStr">
         <is>
-          <t>B2</t>
+          <t>B1</t>
         </is>
       </c>
       <c r="C71" s="6" t="inlineStr">
         <is>
-          <t>anatomy</t>
+          <t>microbiology</t>
         </is>
       </c>
       <c r="D71" s="6" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E71" s="7" t="inlineStr">
         <is>
-          <t>13/11/2025</t>
+          <t>12/11/2025</t>
         </is>
       </c>
       <c r="F71" s="8" t="inlineStr">
         <is>
-          <t>08:00:00</t>
+          <t>14:00:00</t>
         </is>
       </c>
       <c r="G71" s="9" t="n">
@@ -2975,12 +2975,12 @@
       </c>
       <c r="B72" s="2" t="inlineStr">
         <is>
-          <t>B2</t>
+          <t>B1</t>
         </is>
       </c>
       <c r="C72" s="2" t="inlineStr">
         <is>
-          <t>biochemistry lab/cbl</t>
+          <t>parasitology sgd/pos</t>
         </is>
       </c>
       <c r="D72" s="2" t="inlineStr">
@@ -2990,7 +2990,7 @@
       </c>
       <c r="E72" s="3" t="inlineStr">
         <is>
-          <t>10/11/2025</t>
+          <t>19/11/2025</t>
         </is>
       </c>
       <c r="F72" s="4" t="inlineStr">
@@ -2999,7 +2999,7 @@
         </is>
       </c>
       <c r="G72" s="5" t="n">
-        <v>120</v>
+        <v>90</v>
       </c>
     </row>
     <row r="73">
@@ -3010,27 +3010,27 @@
       </c>
       <c r="B73" s="6" t="inlineStr">
         <is>
-          <t>B2</t>
+          <t>B1</t>
         </is>
       </c>
       <c r="C73" s="6" t="inlineStr">
         <is>
-          <t>biochemistry lab/cbl</t>
+          <t>pathology lab/museum</t>
         </is>
       </c>
       <c r="D73" s="6" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E73" s="7" t="inlineStr">
         <is>
-          <t>18/11/2025</t>
+          <t>17/11/2025</t>
         </is>
       </c>
       <c r="F73" s="8" t="inlineStr">
         <is>
-          <t>10:00:00</t>
+          <t>12:00:00</t>
         </is>
       </c>
       <c r="G73" s="9" t="n">
@@ -3045,22 +3045,22 @@
       </c>
       <c r="B74" s="2" t="inlineStr">
         <is>
-          <t>B2</t>
+          <t>B1</t>
         </is>
       </c>
       <c r="C74" s="2" t="inlineStr">
         <is>
-          <t>histology</t>
+          <t>pathology lab/museum</t>
         </is>
       </c>
       <c r="D74" s="2" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E74" s="3" t="inlineStr">
         <is>
-          <t>22/10/2025</t>
+          <t>17/11/2025</t>
         </is>
       </c>
       <c r="F74" s="4" t="inlineStr">
@@ -3080,22 +3080,22 @@
       </c>
       <c r="B75" s="6" t="inlineStr">
         <is>
-          <t>B2</t>
+          <t>B1</t>
         </is>
       </c>
       <c r="C75" s="6" t="inlineStr">
         <is>
-          <t>histology</t>
+          <t>pharmacology</t>
         </is>
       </c>
       <c r="D75" s="6" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E75" s="7" t="inlineStr">
         <is>
-          <t>18/11/2025</t>
+          <t>05/11/2025</t>
         </is>
       </c>
       <c r="F75" s="8" t="inlineStr">
@@ -3115,27 +3115,27 @@
       </c>
       <c r="B76" s="2" t="inlineStr">
         <is>
-          <t>B2</t>
+          <t>B1</t>
         </is>
       </c>
       <c r="C76" s="2" t="inlineStr">
         <is>
-          <t>microbiology</t>
+          <t>pharmacology</t>
         </is>
       </c>
       <c r="D76" s="2" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E76" s="3" t="inlineStr">
         <is>
-          <t>12/11/2025</t>
+          <t>19/11/2025</t>
         </is>
       </c>
       <c r="F76" s="4" t="inlineStr">
         <is>
-          <t>12:00:00</t>
+          <t>08:00:00</t>
         </is>
       </c>
       <c r="G76" s="5" t="n">
@@ -3150,12 +3150,12 @@
       </c>
       <c r="B77" s="6" t="inlineStr">
         <is>
-          <t>B2</t>
+          <t>B1</t>
         </is>
       </c>
       <c r="C77" s="6" t="inlineStr">
         <is>
-          <t>pathology lab/museum</t>
+          <t>physiology</t>
         </is>
       </c>
       <c r="D77" s="6" t="inlineStr">
@@ -3165,12 +3165,12 @@
       </c>
       <c r="E77" s="7" t="inlineStr">
         <is>
-          <t>17/11/2025</t>
+          <t>10/11/2025</t>
         </is>
       </c>
       <c r="F77" s="8" t="inlineStr">
         <is>
-          <t>14:00:00</t>
+          <t>10:00:00</t>
         </is>
       </c>
       <c r="G77" s="9" t="n">
@@ -3185,12 +3185,12 @@
       </c>
       <c r="B78" s="2" t="inlineStr">
         <is>
-          <t>B2</t>
+          <t>B1</t>
         </is>
       </c>
       <c r="C78" s="2" t="inlineStr">
         <is>
-          <t>pathology lab/museum</t>
+          <t>physiology</t>
         </is>
       </c>
       <c r="D78" s="2" t="inlineStr">
@@ -3200,16 +3200,16 @@
       </c>
       <c r="E78" s="3" t="inlineStr">
         <is>
-          <t>17/11/2025</t>
+          <t>19/11/2025</t>
         </is>
       </c>
       <c r="F78" s="4" t="inlineStr">
         <is>
-          <t>12:00:00</t>
+          <t>10:00:00</t>
         </is>
       </c>
       <c r="G78" s="5" t="n">
-        <v>120</v>
+        <v>90</v>
       </c>
     </row>
     <row r="79">
@@ -3225,7 +3225,7 @@
       </c>
       <c r="C79" s="6" t="inlineStr">
         <is>
-          <t>pharmacology</t>
+          <t>anatomy</t>
         </is>
       </c>
       <c r="D79" s="6" t="inlineStr">
@@ -3235,12 +3235,12 @@
       </c>
       <c r="E79" s="7" t="inlineStr">
         <is>
-          <t>05/11/2025</t>
+          <t>20/10/2025</t>
         </is>
       </c>
       <c r="F79" s="8" t="inlineStr">
         <is>
-          <t>14:00:00</t>
+          <t>08:00:00</t>
         </is>
       </c>
       <c r="G79" s="9" t="n">
@@ -3260,7 +3260,7 @@
       </c>
       <c r="C80" s="2" t="inlineStr">
         <is>
-          <t>pharmacology</t>
+          <t>anatomy</t>
         </is>
       </c>
       <c r="D80" s="2" t="inlineStr">
@@ -3270,12 +3270,12 @@
       </c>
       <c r="E80" s="3" t="inlineStr">
         <is>
-          <t>19/11/2025</t>
+          <t>30/10/2025</t>
         </is>
       </c>
       <c r="F80" s="4" t="inlineStr">
         <is>
-          <t>10:00:00</t>
+          <t>08:00:00</t>
         </is>
       </c>
       <c r="G80" s="5" t="n">
@@ -3295,17 +3295,17 @@
       </c>
       <c r="C81" s="6" t="inlineStr">
         <is>
-          <t>physiology</t>
+          <t>anatomy</t>
         </is>
       </c>
       <c r="D81" s="6" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E81" s="7" t="inlineStr">
         <is>
-          <t>10/11/2025</t>
+          <t>13/11/2025</t>
         </is>
       </c>
       <c r="F81" s="8" t="inlineStr">
@@ -3325,12 +3325,12 @@
       </c>
       <c r="B82" s="2" t="inlineStr">
         <is>
-          <t>B3</t>
+          <t>B2</t>
         </is>
       </c>
       <c r="C82" s="2" t="inlineStr">
         <is>
-          <t>anatomy</t>
+          <t>biochemistry lab/cbl</t>
         </is>
       </c>
       <c r="D82" s="2" t="inlineStr">
@@ -3340,7 +3340,7 @@
       </c>
       <c r="E82" s="3" t="inlineStr">
         <is>
-          <t>23/10/2025</t>
+          <t>10/11/2025</t>
         </is>
       </c>
       <c r="F82" s="4" t="inlineStr">
@@ -3360,12 +3360,12 @@
       </c>
       <c r="B83" s="6" t="inlineStr">
         <is>
-          <t>B3</t>
+          <t>B2</t>
         </is>
       </c>
       <c r="C83" s="6" t="inlineStr">
         <is>
-          <t>anatomy</t>
+          <t>biochemistry lab/cbl</t>
         </is>
       </c>
       <c r="D83" s="6" t="inlineStr">
@@ -3375,12 +3375,12 @@
       </c>
       <c r="E83" s="7" t="inlineStr">
         <is>
-          <t>01/11/2025</t>
+          <t>18/11/2025</t>
         </is>
       </c>
       <c r="F83" s="8" t="inlineStr">
         <is>
-          <t>12:00:00</t>
+          <t>10:00:00</t>
         </is>
       </c>
       <c r="G83" s="9" t="n">
@@ -3395,22 +3395,22 @@
       </c>
       <c r="B84" s="2" t="inlineStr">
         <is>
-          <t>B3</t>
+          <t>B2</t>
         </is>
       </c>
       <c r="C84" s="2" t="inlineStr">
         <is>
-          <t>anatomy</t>
+          <t>histology</t>
         </is>
       </c>
       <c r="D84" s="2" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E84" s="3" t="inlineStr">
         <is>
-          <t>12/11/2025</t>
+          <t>22/10/2025</t>
         </is>
       </c>
       <c r="F84" s="4" t="inlineStr">
@@ -3430,22 +3430,22 @@
       </c>
       <c r="B85" s="6" t="inlineStr">
         <is>
-          <t>B3</t>
+          <t>B2</t>
         </is>
       </c>
       <c r="C85" s="6" t="inlineStr">
         <is>
-          <t>biochemistry lab/cbl</t>
+          <t>histology</t>
         </is>
       </c>
       <c r="D85" s="6" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E85" s="7" t="inlineStr">
         <is>
-          <t>12/11/2025</t>
+          <t>18/11/2025</t>
         </is>
       </c>
       <c r="F85" s="8" t="inlineStr">
@@ -3465,22 +3465,22 @@
       </c>
       <c r="B86" s="2" t="inlineStr">
         <is>
-          <t>B3</t>
+          <t>B2</t>
         </is>
       </c>
       <c r="C86" s="2" t="inlineStr">
         <is>
-          <t>biochemistry lab/cbl</t>
+          <t>microbiology</t>
         </is>
       </c>
       <c r="D86" s="2" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E86" s="3" t="inlineStr">
         <is>
-          <t>18/11/2025</t>
+          <t>12/11/2025</t>
         </is>
       </c>
       <c r="F86" s="4" t="inlineStr">
@@ -3500,12 +3500,12 @@
       </c>
       <c r="B87" s="6" t="inlineStr">
         <is>
-          <t>B3</t>
+          <t>B2</t>
         </is>
       </c>
       <c r="C87" s="6" t="inlineStr">
         <is>
-          <t>histology</t>
+          <t>parasitology sgd/pos</t>
         </is>
       </c>
       <c r="D87" s="6" t="inlineStr">
@@ -3515,7 +3515,7 @@
       </c>
       <c r="E87" s="7" t="inlineStr">
         <is>
-          <t>23/10/2025</t>
+          <t>19/11/2025</t>
         </is>
       </c>
       <c r="F87" s="8" t="inlineStr">
@@ -3524,7 +3524,7 @@
         </is>
       </c>
       <c r="G87" s="9" t="n">
-        <v>120</v>
+        <v>90</v>
       </c>
     </row>
     <row r="88">
@@ -3535,12 +3535,12 @@
       </c>
       <c r="B88" s="2" t="inlineStr">
         <is>
-          <t>B3</t>
+          <t>B2</t>
         </is>
       </c>
       <c r="C88" s="2" t="inlineStr">
         <is>
-          <t>microbiology</t>
+          <t>pathology lab/museum</t>
         </is>
       </c>
       <c r="D88" s="2" t="inlineStr">
@@ -3550,12 +3550,12 @@
       </c>
       <c r="E88" s="3" t="inlineStr">
         <is>
-          <t>13/11/2025</t>
+          <t>17/11/2025</t>
         </is>
       </c>
       <c r="F88" s="4" t="inlineStr">
         <is>
-          <t>08:00:00</t>
+          <t>14:00:00</t>
         </is>
       </c>
       <c r="G88" s="5" t="n">
@@ -3570,12 +3570,12 @@
       </c>
       <c r="B89" s="6" t="inlineStr">
         <is>
-          <t>B3</t>
+          <t>B2</t>
         </is>
       </c>
       <c r="C89" s="6" t="inlineStr">
         <is>
-          <t>microbiology</t>
+          <t>pathology lab/museum</t>
         </is>
       </c>
       <c r="D89" s="6" t="inlineStr">
@@ -3585,12 +3585,12 @@
       </c>
       <c r="E89" s="7" t="inlineStr">
         <is>
-          <t>15/11/2025</t>
+          <t>17/11/2025</t>
         </is>
       </c>
       <c r="F89" s="8" t="inlineStr">
         <is>
-          <t>14:00:00</t>
+          <t>12:00:00</t>
         </is>
       </c>
       <c r="G89" s="9" t="n">
@@ -3605,12 +3605,12 @@
       </c>
       <c r="B90" s="2" t="inlineStr">
         <is>
-          <t>B3</t>
+          <t>B2</t>
         </is>
       </c>
       <c r="C90" s="2" t="inlineStr">
         <is>
-          <t>pathology lab/museum</t>
+          <t>pharmacology</t>
         </is>
       </c>
       <c r="D90" s="2" t="inlineStr">
@@ -3620,12 +3620,12 @@
       </c>
       <c r="E90" s="3" t="inlineStr">
         <is>
-          <t>19/11/2025</t>
+          <t>05/11/2025</t>
         </is>
       </c>
       <c r="F90" s="4" t="inlineStr">
         <is>
-          <t>12:00:00</t>
+          <t>14:00:00</t>
         </is>
       </c>
       <c r="G90" s="5" t="n">
@@ -3640,12 +3640,12 @@
       </c>
       <c r="B91" s="6" t="inlineStr">
         <is>
-          <t>B3</t>
+          <t>B2</t>
         </is>
       </c>
       <c r="C91" s="6" t="inlineStr">
         <is>
-          <t>pathology lab/museum</t>
+          <t>pharmacology</t>
         </is>
       </c>
       <c r="D91" s="6" t="inlineStr">
@@ -3660,7 +3660,7 @@
       </c>
       <c r="F91" s="8" t="inlineStr">
         <is>
-          <t>14:00:00</t>
+          <t>10:00:00</t>
         </is>
       </c>
       <c r="G91" s="9" t="n">
@@ -3675,12 +3675,12 @@
       </c>
       <c r="B92" s="2" t="inlineStr">
         <is>
-          <t>B3</t>
+          <t>B2</t>
         </is>
       </c>
       <c r="C92" s="2" t="inlineStr">
         <is>
-          <t>pharmacology</t>
+          <t>physiology</t>
         </is>
       </c>
       <c r="D92" s="2" t="inlineStr">
@@ -3690,12 +3690,12 @@
       </c>
       <c r="E92" s="3" t="inlineStr">
         <is>
-          <t>04/11/2025</t>
+          <t>10/11/2025</t>
         </is>
       </c>
       <c r="F92" s="4" t="inlineStr">
         <is>
-          <t>12:00:00</t>
+          <t>08:00:00</t>
         </is>
       </c>
       <c r="G92" s="5" t="n">
@@ -3710,12 +3710,12 @@
       </c>
       <c r="B93" s="6" t="inlineStr">
         <is>
-          <t>B3</t>
+          <t>B2</t>
         </is>
       </c>
       <c r="C93" s="6" t="inlineStr">
         <is>
-          <t>pharmacology</t>
+          <t>physiology</t>
         </is>
       </c>
       <c r="D93" s="6" t="inlineStr">
@@ -3725,16 +3725,16 @@
       </c>
       <c r="E93" s="7" t="inlineStr">
         <is>
-          <t>16/11/2025</t>
+          <t>19/11/2025</t>
         </is>
       </c>
       <c r="F93" s="8" t="inlineStr">
         <is>
-          <t>12:00:00</t>
+          <t>08:00:00</t>
         </is>
       </c>
       <c r="G93" s="9" t="n">
-        <v>120</v>
+        <v>90</v>
       </c>
     </row>
     <row r="94">
@@ -3750,7 +3750,7 @@
       </c>
       <c r="C94" s="2" t="inlineStr">
         <is>
-          <t>physiology</t>
+          <t>anatomy</t>
         </is>
       </c>
       <c r="D94" s="2" t="inlineStr">
@@ -3760,7 +3760,7 @@
       </c>
       <c r="E94" s="3" t="inlineStr">
         <is>
-          <t>13/11/2025</t>
+          <t>23/10/2025</t>
         </is>
       </c>
       <c r="F94" s="4" t="inlineStr">
@@ -3780,7 +3780,7 @@
       </c>
       <c r="B95" s="6" t="inlineStr">
         <is>
-          <t>B4</t>
+          <t>B3</t>
         </is>
       </c>
       <c r="C95" s="6" t="inlineStr">
@@ -3790,17 +3790,17 @@
       </c>
       <c r="D95" s="6" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E95" s="7" t="inlineStr">
         <is>
-          <t>23/10/2025</t>
+          <t>01/11/2025</t>
         </is>
       </c>
       <c r="F95" s="8" t="inlineStr">
         <is>
-          <t>08:00:00</t>
+          <t>12:00:00</t>
         </is>
       </c>
       <c r="G95" s="9" t="n">
@@ -3815,7 +3815,7 @@
       </c>
       <c r="B96" s="2" t="inlineStr">
         <is>
-          <t>B4</t>
+          <t>B3</t>
         </is>
       </c>
       <c r="C96" s="2" t="inlineStr">
@@ -3825,12 +3825,12 @@
       </c>
       <c r="D96" s="2" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E96" s="3" t="inlineStr">
         <is>
-          <t>01/11/2025</t>
+          <t>12/11/2025</t>
         </is>
       </c>
       <c r="F96" s="4" t="inlineStr">
@@ -3850,27 +3850,27 @@
       </c>
       <c r="B97" s="6" t="inlineStr">
         <is>
-          <t>B4</t>
+          <t>B3</t>
         </is>
       </c>
       <c r="C97" s="6" t="inlineStr">
         <is>
-          <t>anatomy</t>
+          <t>biochemistry lab/cbl</t>
         </is>
       </c>
       <c r="D97" s="6" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E97" s="7" t="inlineStr">
         <is>
-          <t>10/11/2025</t>
+          <t>12/11/2025</t>
         </is>
       </c>
       <c r="F97" s="8" t="inlineStr">
         <is>
-          <t>10:00:00</t>
+          <t>12:00:00</t>
         </is>
       </c>
       <c r="G97" s="9" t="n">
@@ -3885,7 +3885,7 @@
       </c>
       <c r="B98" s="2" t="inlineStr">
         <is>
-          <t>B4</t>
+          <t>B3</t>
         </is>
       </c>
       <c r="C98" s="2" t="inlineStr">
@@ -3895,17 +3895,17 @@
       </c>
       <c r="D98" s="2" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E98" s="3" t="inlineStr">
         <is>
-          <t>12/11/2025</t>
+          <t>18/11/2025</t>
         </is>
       </c>
       <c r="F98" s="4" t="inlineStr">
         <is>
-          <t>14:00:00</t>
+          <t>12:00:00</t>
         </is>
       </c>
       <c r="G98" s="5" t="n">
@@ -3920,27 +3920,27 @@
       </c>
       <c r="B99" s="6" t="inlineStr">
         <is>
-          <t>B4</t>
+          <t>B3</t>
         </is>
       </c>
       <c r="C99" s="6" t="inlineStr">
         <is>
-          <t>biochemistry lab/cbl</t>
+          <t>histology</t>
         </is>
       </c>
       <c r="D99" s="6" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E99" s="7" t="inlineStr">
         <is>
-          <t>18/11/2025</t>
+          <t>23/10/2025</t>
         </is>
       </c>
       <c r="F99" s="8" t="inlineStr">
         <is>
-          <t>14:00:00</t>
+          <t>08:00:00</t>
         </is>
       </c>
       <c r="G99" s="9" t="n">
@@ -3955,12 +3955,12 @@
       </c>
       <c r="B100" s="2" t="inlineStr">
         <is>
-          <t>B4</t>
+          <t>B3</t>
         </is>
       </c>
       <c r="C100" s="2" t="inlineStr">
         <is>
-          <t>histology</t>
+          <t>microbiology</t>
         </is>
       </c>
       <c r="D100" s="2" t="inlineStr">
@@ -3970,12 +3970,12 @@
       </c>
       <c r="E100" s="3" t="inlineStr">
         <is>
-          <t>23/10/2025</t>
+          <t>13/11/2025</t>
         </is>
       </c>
       <c r="F100" s="4" t="inlineStr">
         <is>
-          <t>10:00:00</t>
+          <t>08:00:00</t>
         </is>
       </c>
       <c r="G100" s="5" t="n">
@@ -3990,7 +3990,7 @@
       </c>
       <c r="B101" s="6" t="inlineStr">
         <is>
-          <t>B4</t>
+          <t>B3</t>
         </is>
       </c>
       <c r="C101" s="6" t="inlineStr">
@@ -4000,17 +4000,17 @@
       </c>
       <c r="D101" s="6" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E101" s="7" t="inlineStr">
         <is>
-          <t>13/11/2025</t>
+          <t>15/11/2025</t>
         </is>
       </c>
       <c r="F101" s="8" t="inlineStr">
         <is>
-          <t>10:00:00</t>
+          <t>14:00:00</t>
         </is>
       </c>
       <c r="G101" s="9" t="n">
@@ -4025,31 +4025,31 @@
       </c>
       <c r="B102" s="2" t="inlineStr">
         <is>
-          <t>B4</t>
+          <t>B3</t>
         </is>
       </c>
       <c r="C102" s="2" t="inlineStr">
         <is>
-          <t>microbiology</t>
+          <t>parasitology sgd/pos</t>
         </is>
       </c>
       <c r="D102" s="2" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E102" s="3" t="inlineStr">
         <is>
-          <t>15/11/2025</t>
+          <t>16/11/2025</t>
         </is>
       </c>
       <c r="F102" s="4" t="inlineStr">
         <is>
-          <t>12:00:00</t>
+          <t>14:00:00</t>
         </is>
       </c>
       <c r="G102" s="5" t="n">
-        <v>120</v>
+        <v>90</v>
       </c>
     </row>
     <row r="103">
@@ -4060,12 +4060,12 @@
       </c>
       <c r="B103" s="6" t="inlineStr">
         <is>
-          <t>B4</t>
+          <t>B3</t>
         </is>
       </c>
       <c r="C103" s="6" t="inlineStr">
         <is>
-          <t>parasitology sgd/pos</t>
+          <t>pathology lab/museum</t>
         </is>
       </c>
       <c r="D103" s="6" t="inlineStr">
@@ -4075,7 +4075,7 @@
       </c>
       <c r="E103" s="7" t="inlineStr">
         <is>
-          <t>16/11/2025</t>
+          <t>19/11/2025</t>
         </is>
       </c>
       <c r="F103" s="8" t="inlineStr">
@@ -4084,7 +4084,7 @@
         </is>
       </c>
       <c r="G103" s="9" t="n">
-        <v>90</v>
+        <v>120</v>
       </c>
     </row>
     <row r="104">
@@ -4095,7 +4095,7 @@
       </c>
       <c r="B104" s="2" t="inlineStr">
         <is>
-          <t>B4</t>
+          <t>B3</t>
         </is>
       </c>
       <c r="C104" s="2" t="inlineStr">
@@ -4105,7 +4105,7 @@
       </c>
       <c r="D104" s="2" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E104" s="3" t="inlineStr">
@@ -4130,22 +4130,22 @@
       </c>
       <c r="B105" s="6" t="inlineStr">
         <is>
-          <t>B4</t>
+          <t>B3</t>
         </is>
       </c>
       <c r="C105" s="6" t="inlineStr">
         <is>
-          <t>pathology lab/museum</t>
+          <t>pharmacology</t>
         </is>
       </c>
       <c r="D105" s="6" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E105" s="7" t="inlineStr">
         <is>
-          <t>19/11/2025</t>
+          <t>04/11/2025</t>
         </is>
       </c>
       <c r="F105" s="8" t="inlineStr">
@@ -4165,7 +4165,7 @@
       </c>
       <c r="B106" s="2" t="inlineStr">
         <is>
-          <t>B4</t>
+          <t>B3</t>
         </is>
       </c>
       <c r="C106" s="2" t="inlineStr">
@@ -4175,17 +4175,17 @@
       </c>
       <c r="D106" s="2" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E106" s="3" t="inlineStr">
         <is>
-          <t>04/11/2025</t>
+          <t>16/11/2025</t>
         </is>
       </c>
       <c r="F106" s="4" t="inlineStr">
         <is>
-          <t>14:00:00</t>
+          <t>12:00:00</t>
         </is>
       </c>
       <c r="G106" s="5" t="n">
@@ -4200,27 +4200,27 @@
       </c>
       <c r="B107" s="6" t="inlineStr">
         <is>
-          <t>B4</t>
+          <t>B3</t>
         </is>
       </c>
       <c r="C107" s="6" t="inlineStr">
         <is>
-          <t>pharmacology</t>
+          <t>physiology</t>
         </is>
       </c>
       <c r="D107" s="6" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E107" s="7" t="inlineStr">
         <is>
-          <t>16/11/2025</t>
+          <t>13/11/2025</t>
         </is>
       </c>
       <c r="F107" s="8" t="inlineStr">
         <is>
-          <t>14:00:00</t>
+          <t>10:00:00</t>
         </is>
       </c>
       <c r="G107" s="9" t="n">
@@ -4235,31 +4235,556 @@
       </c>
       <c r="B108" s="2" t="inlineStr">
         <is>
+          <t>B3</t>
+        </is>
+      </c>
+      <c r="C108" s="2" t="inlineStr">
+        <is>
+          <t>physiology</t>
+        </is>
+      </c>
+      <c r="D108" s="2" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="E108" s="3" t="inlineStr">
+        <is>
+          <t>16/11/2025</t>
+        </is>
+      </c>
+      <c r="F108" s="4" t="inlineStr">
+        <is>
+          <t>14:00:00</t>
+        </is>
+      </c>
+      <c r="G108" s="5" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" s="6" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="B109" s="6" t="inlineStr">
+        <is>
           <t>B4</t>
         </is>
       </c>
-      <c r="C108" s="2" t="inlineStr">
+      <c r="C109" s="6" t="inlineStr">
+        <is>
+          <t>anatomy</t>
+        </is>
+      </c>
+      <c r="D109" s="6" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E109" s="7" t="inlineStr">
+        <is>
+          <t>23/10/2025</t>
+        </is>
+      </c>
+      <c r="F109" s="8" t="inlineStr">
+        <is>
+          <t>08:00:00</t>
+        </is>
+      </c>
+      <c r="G109" s="9" t="n">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" s="2" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="B110" s="2" t="inlineStr">
+        <is>
+          <t>B4</t>
+        </is>
+      </c>
+      <c r="C110" s="2" t="inlineStr">
+        <is>
+          <t>anatomy</t>
+        </is>
+      </c>
+      <c r="D110" s="2" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="E110" s="3" t="inlineStr">
+        <is>
+          <t>01/11/2025</t>
+        </is>
+      </c>
+      <c r="F110" s="4" t="inlineStr">
+        <is>
+          <t>14:00:00</t>
+        </is>
+      </c>
+      <c r="G110" s="5" t="n">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" s="6" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="B111" s="6" t="inlineStr">
+        <is>
+          <t>B4</t>
+        </is>
+      </c>
+      <c r="C111" s="6" t="inlineStr">
+        <is>
+          <t>anatomy</t>
+        </is>
+      </c>
+      <c r="D111" s="6" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="E111" s="7" t="inlineStr">
+        <is>
+          <t>10/11/2025</t>
+        </is>
+      </c>
+      <c r="F111" s="8" t="inlineStr">
+        <is>
+          <t>10:00:00</t>
+        </is>
+      </c>
+      <c r="G111" s="9" t="n">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" s="2" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="B112" s="2" t="inlineStr">
+        <is>
+          <t>B4</t>
+        </is>
+      </c>
+      <c r="C112" s="2" t="inlineStr">
+        <is>
+          <t>biochemistry lab/cbl</t>
+        </is>
+      </c>
+      <c r="D112" s="2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E112" s="3" t="inlineStr">
+        <is>
+          <t>12/11/2025</t>
+        </is>
+      </c>
+      <c r="F112" s="4" t="inlineStr">
+        <is>
+          <t>14:00:00</t>
+        </is>
+      </c>
+      <c r="G112" s="5" t="n">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" s="6" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="B113" s="6" t="inlineStr">
+        <is>
+          <t>B4</t>
+        </is>
+      </c>
+      <c r="C113" s="6" t="inlineStr">
+        <is>
+          <t>biochemistry lab/cbl</t>
+        </is>
+      </c>
+      <c r="D113" s="6" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="E113" s="7" t="inlineStr">
+        <is>
+          <t>18/11/2025</t>
+        </is>
+      </c>
+      <c r="F113" s="8" t="inlineStr">
+        <is>
+          <t>14:00:00</t>
+        </is>
+      </c>
+      <c r="G113" s="9" t="n">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" s="2" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="B114" s="2" t="inlineStr">
+        <is>
+          <t>B4</t>
+        </is>
+      </c>
+      <c r="C114" s="2" t="inlineStr">
+        <is>
+          <t>histology</t>
+        </is>
+      </c>
+      <c r="D114" s="2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E114" s="3" t="inlineStr">
+        <is>
+          <t>23/10/2025</t>
+        </is>
+      </c>
+      <c r="F114" s="4" t="inlineStr">
+        <is>
+          <t>10:00:00</t>
+        </is>
+      </c>
+      <c r="G114" s="5" t="n">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" s="6" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="B115" s="6" t="inlineStr">
+        <is>
+          <t>B4</t>
+        </is>
+      </c>
+      <c r="C115" s="6" t="inlineStr">
+        <is>
+          <t>microbiology</t>
+        </is>
+      </c>
+      <c r="D115" s="6" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E115" s="7" t="inlineStr">
+        <is>
+          <t>13/11/2025</t>
+        </is>
+      </c>
+      <c r="F115" s="8" t="inlineStr">
+        <is>
+          <t>10:00:00</t>
+        </is>
+      </c>
+      <c r="G115" s="9" t="n">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" s="2" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="B116" s="2" t="inlineStr">
+        <is>
+          <t>B4</t>
+        </is>
+      </c>
+      <c r="C116" s="2" t="inlineStr">
+        <is>
+          <t>microbiology</t>
+        </is>
+      </c>
+      <c r="D116" s="2" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="E116" s="3" t="inlineStr">
+        <is>
+          <t>15/11/2025</t>
+        </is>
+      </c>
+      <c r="F116" s="4" t="inlineStr">
+        <is>
+          <t>12:00:00</t>
+        </is>
+      </c>
+      <c r="G116" s="5" t="n">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" s="6" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="B117" s="6" t="inlineStr">
+        <is>
+          <t>B4</t>
+        </is>
+      </c>
+      <c r="C117" s="6" t="inlineStr">
+        <is>
+          <t>parasitology sgd/pos</t>
+        </is>
+      </c>
+      <c r="D117" s="6" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E117" s="7" t="inlineStr">
+        <is>
+          <t>16/11/2025</t>
+        </is>
+      </c>
+      <c r="F117" s="8" t="inlineStr">
+        <is>
+          <t>12:00:00</t>
+        </is>
+      </c>
+      <c r="G117" s="9" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" s="2" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="B118" s="2" t="inlineStr">
+        <is>
+          <t>B4</t>
+        </is>
+      </c>
+      <c r="C118" s="2" t="inlineStr">
+        <is>
+          <t>pathology lab/museum</t>
+        </is>
+      </c>
+      <c r="D118" s="2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E118" s="3" t="inlineStr">
+        <is>
+          <t>19/11/2025</t>
+        </is>
+      </c>
+      <c r="F118" s="4" t="inlineStr">
+        <is>
+          <t>14:00:00</t>
+        </is>
+      </c>
+      <c r="G118" s="5" t="n">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" s="6" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="B119" s="6" t="inlineStr">
+        <is>
+          <t>B4</t>
+        </is>
+      </c>
+      <c r="C119" s="6" t="inlineStr">
+        <is>
+          <t>pathology lab/museum</t>
+        </is>
+      </c>
+      <c r="D119" s="6" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="E119" s="7" t="inlineStr">
+        <is>
+          <t>19/11/2025</t>
+        </is>
+      </c>
+      <c r="F119" s="8" t="inlineStr">
+        <is>
+          <t>12:00:00</t>
+        </is>
+      </c>
+      <c r="G119" s="9" t="n">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" s="2" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="B120" s="2" t="inlineStr">
+        <is>
+          <t>B4</t>
+        </is>
+      </c>
+      <c r="C120" s="2" t="inlineStr">
+        <is>
+          <t>pharmacology</t>
+        </is>
+      </c>
+      <c r="D120" s="2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E120" s="3" t="inlineStr">
+        <is>
+          <t>04/11/2025</t>
+        </is>
+      </c>
+      <c r="F120" s="4" t="inlineStr">
+        <is>
+          <t>14:00:00</t>
+        </is>
+      </c>
+      <c r="G120" s="5" t="n">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" s="6" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="B121" s="6" t="inlineStr">
+        <is>
+          <t>B4</t>
+        </is>
+      </c>
+      <c r="C121" s="6" t="inlineStr">
+        <is>
+          <t>pharmacology</t>
+        </is>
+      </c>
+      <c r="D121" s="6" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="E121" s="7" t="inlineStr">
+        <is>
+          <t>16/11/2025</t>
+        </is>
+      </c>
+      <c r="F121" s="8" t="inlineStr">
+        <is>
+          <t>14:00:00</t>
+        </is>
+      </c>
+      <c r="G121" s="9" t="n">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" s="2" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="B122" s="2" t="inlineStr">
+        <is>
+          <t>B4</t>
+        </is>
+      </c>
+      <c r="C122" s="2" t="inlineStr">
         <is>
           <t>physiology</t>
         </is>
       </c>
-      <c r="D108" s="2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="E108" s="3" t="inlineStr">
+      <c r="D122" s="2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E122" s="3" t="inlineStr">
         <is>
           <t>13/11/2025</t>
         </is>
       </c>
-      <c r="F108" s="4" t="inlineStr">
+      <c r="F122" s="4" t="inlineStr">
         <is>
           <t>08:00:00</t>
         </is>
       </c>
-      <c r="G108" s="5" t="n">
-        <v>120</v>
+      <c r="G122" s="5" t="n">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" s="6" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="B123" s="6" t="inlineStr">
+        <is>
+          <t>B4</t>
+        </is>
+      </c>
+      <c r="C123" s="6" t="inlineStr">
+        <is>
+          <t>physiology</t>
+        </is>
+      </c>
+      <c r="D123" s="6" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="E123" s="7" t="inlineStr">
+        <is>
+          <t>16/11/2025</t>
+        </is>
+      </c>
+      <c r="F123" s="8" t="inlineStr">
+        <is>
+          <t>12:00:00</t>
+        </is>
+      </c>
+      <c r="G123" s="9" t="n">
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>